<commit_message>
final del proceso de facturacion
</commit_message>
<xml_diff>
--- a/public/files/formato-val-minsur.xlsx
+++ b/public/files/formato-val-minsur.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Valorizacion" sheetId="1" r:id="rId1"/>
+    <sheet name="Participantes" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>INVERITAS GLOBAL HOLDINGS PERU S.A</t>
   </si>
@@ -135,6 +136,36 @@
   </si>
   <si>
     <t>Servicio por Cursos Obligatorios y/o Riesgos Críticos</t>
+  </si>
+  <si>
+    <t>DNI</t>
+  </si>
+  <si>
+    <t>Apellido Materno</t>
+  </si>
+  <si>
+    <t>Apellido Paterno</t>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Cargo</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>Empresa</t>
+  </si>
+  <si>
+    <t>Curso</t>
+  </si>
+  <si>
+    <t>Horas</t>
+  </si>
+  <si>
+    <t>Fecha</t>
   </si>
 </sst>
 </file>
@@ -356,7 +387,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -393,6 +424,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="46">
     <border>
@@ -965,7 +1002,7 @@
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="169" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="145">
+  <cellXfs count="147">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1395,6 +1432,8 @@
     <xf numFmtId="0" fontId="13" fillId="4" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Millares 2" xfId="3"/>
@@ -1899,8 +1938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2364,4 +2403,64 @@
   <pageSetup scale="80" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:J1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" customWidth="1"/>
+    <col min="8" max="8" width="34.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="145" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="145" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="145" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="145" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="145" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="145" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="145" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="145" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" s="145" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" s="145" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="146"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
subir pedido de vega
</commit_message>
<xml_diff>
--- a/public/files/formato-val-minsur.xlsx
+++ b/public/files/formato-val-minsur.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Valorizacion" sheetId="1" r:id="rId1"/>
@@ -1303,6 +1303,8 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="2" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1432,8 +1434,6 @@
     <xf numFmtId="0" fontId="13" fillId="4" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Millares 2" xfId="3"/>
@@ -1475,7 +1475,7 @@
         <xdr:cNvPr id="2" name="1 Imagen">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6CAFA8D0-A6F4-4BAC-B3F9-9774BE5DDCDF}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CAFA8D0-A6F4-4BAC-B3F9-9774BE5DDCDF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1549,7 +1549,7 @@
         <xdr:cNvPr id="3" name="9 Imagen" descr="http://beta.sefinanzas.pe/media/BAhbBlsHOgZmSSIhMjAxNC8wMS8yOS8xNV8yNF81OF80OTJfZmlsZQY6BkVU.jpeg">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{36291846-D2F5-43D9-83CC-51A397DB100C}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{36291846-D2F5-43D9-83CC-51A397DB100C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1938,8 +1938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H37"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1963,48 +1963,48 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="117" t="s">
+      <c r="B2" s="119" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="118"/>
-      <c r="D2" s="118"/>
-      <c r="E2" s="118"/>
-      <c r="F2" s="118"/>
-      <c r="G2" s="118"/>
-      <c r="H2" s="119"/>
+      <c r="C2" s="120"/>
+      <c r="D2" s="120"/>
+      <c r="E2" s="120"/>
+      <c r="F2" s="120"/>
+      <c r="G2" s="120"/>
+      <c r="H2" s="121"/>
     </row>
     <row r="3" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="108" t="s">
+      <c r="B3" s="110" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="109"/>
-      <c r="D3" s="109"/>
-      <c r="E3" s="109"/>
-      <c r="F3" s="109"/>
-      <c r="G3" s="109"/>
-      <c r="H3" s="110"/>
+      <c r="C3" s="111"/>
+      <c r="D3" s="111"/>
+      <c r="E3" s="111"/>
+      <c r="F3" s="111"/>
+      <c r="G3" s="111"/>
+      <c r="H3" s="112"/>
     </row>
     <row r="4" spans="2:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="120" t="s">
+      <c r="B4" s="122" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="121"/>
-      <c r="D4" s="121"/>
-      <c r="E4" s="121"/>
-      <c r="F4" s="121"/>
-      <c r="G4" s="121"/>
-      <c r="H4" s="122"/>
+      <c r="C4" s="123"/>
+      <c r="D4" s="123"/>
+      <c r="E4" s="123"/>
+      <c r="F4" s="123"/>
+      <c r="G4" s="123"/>
+      <c r="H4" s="124"/>
     </row>
     <row r="5" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="123" t="s">
+      <c r="B5" s="125" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="124"/>
-      <c r="D5" s="124"/>
-      <c r="E5" s="124"/>
-      <c r="F5" s="124"/>
-      <c r="G5" s="124"/>
-      <c r="H5" s="125"/>
+      <c r="C5" s="126"/>
+      <c r="D5" s="126"/>
+      <c r="E5" s="126"/>
+      <c r="F5" s="126"/>
+      <c r="G5" s="126"/>
+      <c r="H5" s="127"/>
     </row>
     <row r="6" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="2"/>
@@ -2084,46 +2084,46 @@
       <c r="B12" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="126" t="s">
+      <c r="C12" s="128" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="127"/>
-      <c r="E12" s="132" t="s">
+      <c r="D12" s="129"/>
+      <c r="E12" s="134" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="133"/>
-      <c r="G12" s="134"/>
+      <c r="F12" s="135"/>
+      <c r="G12" s="136"/>
       <c r="H12" s="30" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="13" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="135" t="s">
+      <c r="B13" s="137" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="128"/>
-      <c r="D13" s="129"/>
-      <c r="E13" s="137" t="s">
+      <c r="C13" s="130"/>
+      <c r="D13" s="131"/>
+      <c r="E13" s="139" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="139" t="s">
+      <c r="F13" s="141" t="s">
         <v>30</v>
       </c>
-      <c r="G13" s="141" t="s">
+      <c r="G13" s="143" t="s">
         <v>16</v>
       </c>
-      <c r="H13" s="143" t="s">
+      <c r="H13" s="145" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="14" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="136"/>
-      <c r="C14" s="130"/>
-      <c r="D14" s="131"/>
-      <c r="E14" s="138"/>
-      <c r="F14" s="140"/>
-      <c r="G14" s="142"/>
-      <c r="H14" s="144"/>
+      <c r="B14" s="138"/>
+      <c r="C14" s="132"/>
+      <c r="D14" s="133"/>
+      <c r="E14" s="140"/>
+      <c r="F14" s="142"/>
+      <c r="G14" s="144"/>
+      <c r="H14" s="146"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="31"/>
@@ -2136,7 +2136,7 @@
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="38">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C16" s="39" t="s">
         <v>18</v>
@@ -2244,24 +2244,24 @@
       </c>
     </row>
     <row r="24" spans="2:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="102"/>
-      <c r="C24" s="103"/>
-      <c r="D24" s="103"/>
-      <c r="E24" s="103"/>
-      <c r="F24" s="103"/>
-      <c r="G24" s="103"/>
-      <c r="H24" s="104"/>
+      <c r="B24" s="104"/>
+      <c r="C24" s="105"/>
+      <c r="D24" s="105"/>
+      <c r="E24" s="105"/>
+      <c r="F24" s="105"/>
+      <c r="G24" s="105"/>
+      <c r="H24" s="106"/>
     </row>
     <row r="25" spans="2:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="105" t="s">
+      <c r="B25" s="107" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="106"/>
-      <c r="D25" s="106"/>
-      <c r="E25" s="106"/>
-      <c r="F25" s="106"/>
-      <c r="G25" s="106"/>
-      <c r="H25" s="107"/>
+      <c r="C25" s="108"/>
+      <c r="D25" s="108"/>
+      <c r="E25" s="108"/>
+      <c r="F25" s="108"/>
+      <c r="G25" s="108"/>
+      <c r="H25" s="109"/>
     </row>
     <row r="26" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="11" t="s">
@@ -2342,12 +2342,12 @@
       <c r="H33" s="92"/>
     </row>
     <row r="34" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B34" s="108" t="s">
+      <c r="B34" s="110" t="s">
         <v>25</v>
       </c>
-      <c r="C34" s="109"/>
-      <c r="D34" s="109"/>
-      <c r="E34" s="110"/>
+      <c r="C34" s="111"/>
+      <c r="D34" s="111"/>
+      <c r="E34" s="112"/>
       <c r="F34" s="93"/>
       <c r="G34" s="89"/>
       <c r="H34" s="92"/>
@@ -2362,24 +2362,24 @@
       <c r="H35" s="98"/>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="111" t="s">
+      <c r="B36" s="113" t="s">
         <v>26</v>
       </c>
-      <c r="C36" s="112"/>
-      <c r="D36" s="112"/>
-      <c r="E36" s="112"/>
-      <c r="F36" s="112"/>
-      <c r="G36" s="112"/>
-      <c r="H36" s="113"/>
+      <c r="C36" s="114"/>
+      <c r="D36" s="114"/>
+      <c r="E36" s="114"/>
+      <c r="F36" s="114"/>
+      <c r="G36" s="114"/>
+      <c r="H36" s="115"/>
     </row>
     <row r="37" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="114"/>
-      <c r="C37" s="115"/>
-      <c r="D37" s="115"/>
-      <c r="E37" s="115"/>
-      <c r="F37" s="115"/>
-      <c r="G37" s="115"/>
-      <c r="H37" s="116"/>
+      <c r="B37" s="116"/>
+      <c r="C37" s="117"/>
+      <c r="D37" s="117"/>
+      <c r="E37" s="117"/>
+      <c r="F37" s="117"/>
+      <c r="G37" s="117"/>
+      <c r="H37" s="118"/>
     </row>
   </sheetData>
   <mergeCells count="15">
@@ -2409,8 +2409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:J1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2425,39 +2425,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="145" t="s">
+      <c r="A1" s="102" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="145" t="s">
+      <c r="B1" s="102" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="145" t="s">
+      <c r="C1" s="102" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="145" t="s">
+      <c r="D1" s="102" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="145" t="s">
+      <c r="E1" s="102" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="145" t="s">
+      <c r="F1" s="102" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="145" t="s">
+      <c r="G1" s="102" t="s">
         <v>41</v>
       </c>
-      <c r="H1" s="145" t="s">
+      <c r="H1" s="102" t="s">
         <v>42</v>
       </c>
-      <c r="I1" s="145" t="s">
+      <c r="I1" s="102" t="s">
         <v>43</v>
       </c>
-      <c r="J1" s="145" t="s">
+      <c r="J1" s="102" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="146"/>
+      <c r="B4" s="103"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
creacion de campo vacantes
</commit_message>
<xml_diff>
--- a/public/files/formato-val-minsur.xlsx
+++ b/public/files/formato-val-minsur.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\minsur\public\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IGH GROUP\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="12585"/>
   </bookViews>
   <sheets>
     <sheet name="Valorizacion" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>INVERITAS GLOBAL HOLDINGS PERU S.A</t>
   </si>
@@ -38,9 +38,6 @@
     <t>AV. LA ENCALADA Nº 1257, OF 801, SANTIAGO DE SURCO - LIMA TELEF: 437-9184</t>
   </si>
   <si>
-    <t>DETALLE DE SERVICIOS</t>
-  </si>
-  <si>
     <t xml:space="preserve">                         RUC N° </t>
   </si>
   <si>
@@ -51,9 +48,6 @@
   </si>
   <si>
     <t>Unidad Minera:</t>
-  </si>
-  <si>
-    <t>Estado de pago:</t>
   </si>
   <si>
     <t xml:space="preserve">Período°: </t>
@@ -87,9 +81,6 @@
     <t>IMPORTE S/</t>
   </si>
   <si>
-    <t xml:space="preserve">Servicio de Inducción y Capacitación en Seguridad y Salud en el Trabajo </t>
-  </si>
-  <si>
     <t>Item del servicio:</t>
   </si>
   <si>
@@ -108,9 +99,6 @@
     <t>Aprovador por Contratista</t>
   </si>
   <si>
-    <t>VICTORIA PECHE</t>
-  </si>
-  <si>
     <t>*Después de revisado y aprobado el presente documento , Enviar escaneado al correo debidamente firmando para adjuntar a la factura.</t>
   </si>
   <si>
@@ -126,15 +114,9 @@
     <t>Cantidad Cobros</t>
   </si>
   <si>
-    <t>Valor Neto a Facturar sin IGV   S/.</t>
-  </si>
-  <si>
     <t xml:space="preserve">CLIENTE: </t>
   </si>
   <si>
-    <t xml:space="preserve"> Servicio de Inducción y Capacitación en Seguridad y Salud en el Trabajo para el personal asignado a la Unidad Minera</t>
-  </si>
-  <si>
     <t>Servicio por Cursos Obligatorios y/o Riesgos Críticos</t>
   </si>
   <si>
@@ -166,6 +148,21 @@
   </si>
   <si>
     <t>Fecha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Servicio de Capacitación en Seguridad y Salud en el Trabajo </t>
+  </si>
+  <si>
+    <t>DETALLE DE VALORIZACION DE SERVICIOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Servicio de  Capacitación en Seguridad y Salud en el Trabajo para el personal asignado a la Unidad Minera</t>
+  </si>
+  <si>
+    <t>Valor Neto a Facturar sin IGV   S/</t>
+  </si>
+  <si>
+    <t>Nro. de Valorizacion:</t>
   </si>
 </sst>
 </file>
@@ -1423,10 +1420,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1595,39 +1592,33 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1552575</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:colOff>1333500</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1829065</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>190</xdr:rowOff>
+      <xdr:colOff>1361869</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>95133</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Imagen 4"/>
+        <xdr:cNvPr id="4" name="Imagen 3"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2828925" y="5800725"/>
-          <a:ext cx="1895740" cy="1362265"/>
+          <a:off x="2609850" y="5934075"/>
+          <a:ext cx="1647619" cy="933333"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1938,8 +1929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1948,8 +1939,8 @@
     <col min="2" max="2" width="14.5703125" customWidth="1"/>
     <col min="3" max="3" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="47.140625" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" customWidth="1"/>
     <col min="7" max="8" width="18" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1986,7 +1977,7 @@
     </row>
     <row r="4" spans="2:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="122" t="s">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="C4" s="123"/>
       <c r="D4" s="123"/>
@@ -1997,7 +1988,7 @@
     </row>
     <row r="5" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="125" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="C5" s="126"/>
       <c r="D5" s="126"/>
@@ -2017,12 +2008,12 @@
     </row>
     <row r="7" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="6" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C7" s="101"/>
       <c r="D7" s="7"/>
       <c r="E7" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
@@ -2033,41 +2024,39 @@
       <c r="C8" s="12"/>
       <c r="D8" s="13"/>
       <c r="E8" s="14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F8" s="15"/>
       <c r="G8" s="16"/>
       <c r="H8" s="17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9" s="99"/>
       <c r="D9" s="19"/>
       <c r="E9" s="20" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="F9" s="21"/>
       <c r="G9" s="16"/>
-      <c r="H9" s="22">
-        <v>1</v>
-      </c>
+      <c r="H9" s="22"/>
     </row>
     <row r="10" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="23" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C10" s="100"/>
       <c r="D10" s="25"/>
       <c r="E10" s="24" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F10" s="24"/>
       <c r="G10" s="26" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H10" s="27"/>
     </row>
@@ -2082,47 +2071,47 @@
     </row>
     <row r="12" spans="2:8" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B12" s="29" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C12" s="128" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D12" s="129"/>
       <c r="E12" s="134" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F12" s="135"/>
       <c r="G12" s="136"/>
       <c r="H12" s="30" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="137" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C13" s="130"/>
       <c r="D13" s="131"/>
-      <c r="E13" s="139" t="s">
+      <c r="E13" s="143" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="141" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" s="139" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" s="145" t="s">
         <v>15</v>
-      </c>
-      <c r="F13" s="141" t="s">
-        <v>30</v>
-      </c>
-      <c r="G13" s="143" t="s">
-        <v>16</v>
-      </c>
-      <c r="H13" s="145" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="14" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="138"/>
       <c r="C14" s="132"/>
       <c r="D14" s="133"/>
-      <c r="E14" s="140"/>
+      <c r="E14" s="144"/>
       <c r="F14" s="142"/>
-      <c r="G14" s="144"/>
+      <c r="G14" s="140"/>
       <c r="H14" s="146"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
@@ -2139,7 +2128,7 @@
         <v>1</v>
       </c>
       <c r="C16" s="39" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="D16" s="40"/>
       <c r="E16" s="41"/>
@@ -2150,7 +2139,7 @@
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="38"/>
       <c r="C17" s="39" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D17" s="40"/>
       <c r="E17" s="41"/>
@@ -2161,14 +2150,14 @@
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="47"/>
       <c r="C18" s="39" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D18" s="40"/>
       <c r="E18" s="48"/>
       <c r="F18" s="49"/>
       <c r="G18" s="45"/>
       <c r="H18" s="46">
-        <f>+F18*G18</f>
+        <f>+F18*E18</f>
         <v>0</v>
       </c>
     </row>
@@ -2185,7 +2174,7 @@
       <c r="B20" s="57"/>
       <c r="C20" s="58"/>
       <c r="D20" s="59" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="E20" s="60">
         <f>SUM(E18:E19)</f>
@@ -2208,7 +2197,7 @@
       <c r="E21" s="68"/>
       <c r="F21" s="69"/>
       <c r="G21" s="70" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="H21" s="71">
         <f>+H20</f>
@@ -2222,7 +2211,7 @@
       <c r="E22" s="68"/>
       <c r="F22" s="72"/>
       <c r="G22" s="73" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="H22" s="71">
         <f>+H21*18%</f>
@@ -2236,7 +2225,7 @@
       <c r="E23" s="68"/>
       <c r="F23" s="74"/>
       <c r="G23" s="75" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="H23" s="76">
         <f>+H21+H22</f>
@@ -2252,9 +2241,9 @@
       <c r="G24" s="105"/>
       <c r="H24" s="106"/>
     </row>
-    <row r="25" spans="2:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:8" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="107" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C25" s="108"/>
       <c r="D25" s="108"/>
@@ -2265,7 +2254,7 @@
     </row>
     <row r="26" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="11" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C26" s="77"/>
       <c r="D26" s="78"/>
@@ -2276,13 +2265,13 @@
     </row>
     <row r="27" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B27" s="83" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C27" s="84"/>
       <c r="D27" s="85"/>
       <c r="E27" s="86"/>
       <c r="F27" s="83" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G27" s="84"/>
       <c r="H27" s="87"/>
@@ -2342,9 +2331,7 @@
       <c r="H33" s="92"/>
     </row>
     <row r="34" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B34" s="110" t="s">
-        <v>25</v>
-      </c>
+      <c r="B34" s="110"/>
       <c r="C34" s="111"/>
       <c r="D34" s="111"/>
       <c r="E34" s="112"/>
@@ -2363,7 +2350,7 @@
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36" s="113" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C36" s="114"/>
       <c r="D36" s="114"/>
@@ -2394,9 +2381,9 @@
     <mergeCell ref="C12:D14"/>
     <mergeCell ref="E12:G12"/>
     <mergeCell ref="B13:B14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="F13:F14"/>
     <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:G14"/>
     <mergeCell ref="H13:H14"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -2426,34 +2413,34 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="102" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="102" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="102" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="102" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="102" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="102" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="102" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="102" t="s">
+      <c r="H1" s="102" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="102" t="s">
+      <c r="I1" s="102" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="102" t="s">
+      <c r="J1" s="102" t="s">
         <v>38</v>
-      </c>
-      <c r="E1" s="102" t="s">
-        <v>39</v>
-      </c>
-      <c r="F1" s="102" t="s">
-        <v>40</v>
-      </c>
-      <c r="G1" s="102" t="s">
-        <v>41</v>
-      </c>
-      <c r="H1" s="102" t="s">
-        <v>42</v>
-      </c>
-      <c r="I1" s="102" t="s">
-        <v>43</v>
-      </c>
-      <c r="J1" s="102" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>